<commit_message>
New catalog including CMIP5 simulations
</commit_message>
<xml_diff>
--- a/catalog.xlsx
+++ b/catalog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="100">
   <si>
     <t>variable_id</t>
   </si>
@@ -22,6 +22,9 @@
     <t>project_id</t>
   </si>
   <si>
+    <t>mip_era</t>
+  </si>
+  <si>
     <t>activity_id</t>
   </si>
   <si>
@@ -55,12 +58,24 @@
     <t>CORDEX</t>
   </si>
   <si>
+    <t>CMIP5</t>
+  </si>
+  <si>
+    <t>CMIP6</t>
+  </si>
+  <si>
     <t>output</t>
   </si>
   <si>
+    <t>DD</t>
+  </si>
+  <si>
     <t>EUR-11</t>
   </si>
   <si>
+    <t>EUR-12</t>
+  </si>
+  <si>
     <t>CLMcom</t>
   </si>
   <si>
@@ -100,9 +115,18 @@
     <t>SMHI</t>
   </si>
   <si>
+    <t>CLMcom-Hereon</t>
+  </si>
+  <si>
+    <t>HCLIMcom-SMHI</t>
+  </si>
+  <si>
     <t>ECMWF-ERAINT</t>
   </si>
   <si>
+    <t>ERA5</t>
+  </si>
+  <si>
     <t>evaluation</t>
   </si>
   <si>
@@ -112,6 +136,9 @@
     <t>r1i1p1</t>
   </si>
   <si>
+    <t>r1i1p1f1</t>
+  </si>
+  <si>
     <t>CCLM4-8-17</t>
   </si>
   <si>
@@ -154,9 +181,24 @@
     <t>RCA4</t>
   </si>
   <si>
+    <t>ICON-CLM-202407-1-1</t>
+  </si>
+  <si>
+    <t>REMO2020</t>
+  </si>
+  <si>
+    <t>HCLIM43-ALADIN</t>
+  </si>
+  <si>
+    <t>RACMO23E</t>
+  </si>
+  <si>
     <t>v1</t>
   </si>
   <si>
+    <t>v1-r1</t>
+  </si>
+  <si>
     <t>fx</t>
   </si>
   <si>
@@ -166,6 +208,9 @@
     <t>day</t>
   </si>
   <si>
+    <t>1hr</t>
+  </si>
+  <si>
     <t>v20140515</t>
   </si>
   <si>
@@ -220,6 +265,18 @@
     <t>v20131026</t>
   </si>
   <si>
+    <t>v20240920</t>
+  </si>
+  <si>
+    <t>v20241120</t>
+  </si>
+  <si>
+    <t>v20241205</t>
+  </si>
+  <si>
+    <t>v20241216</t>
+  </si>
+  <si>
     <t>['orog', 'sftlf']</t>
   </si>
   <si>
@@ -236,6 +293,27 @@
   </si>
   <si>
     <t>['pr', 'tas']</t>
+  </si>
+  <si>
+    <t>['areacella', 'sftlaf', 'mrsofc', 'rootd', 'sftlf', 'sftgif', 'orog', 'sfturf']</t>
+  </si>
+  <si>
+    <t>['hurs', 'pr', 'prsn', 'ps', 'psl', 'tas', 'tasmax', 'tasmin', 'uas', 'vas']</t>
+  </si>
+  <si>
+    <t>['hurs', 'pr', 'prw', 'tas']</t>
+  </si>
+  <si>
+    <t>['pr', 'sfcWindmax', 'snc', 'snd', 'snw', 'tasmax']</t>
+  </si>
+  <si>
+    <t>['areacella', 'orog', 'sftlf', 'sftlaf']</t>
+  </si>
+  <si>
+    <t>['clt', 'rlds', 'rlut', 'rsds', 'sfcWind', 'snc', 'snd', 'snw', 'tas', 'tasmax', 'tasmin', 'uas', 'vas', 'pr']</t>
+  </si>
+  <si>
+    <t>['areacella', 'orog', 'sftlf']</t>
   </si>
 </sst>
 </file>
@@ -593,25 +671,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1"/>
-    <col min="6" max="7" width="23.7109375" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" customWidth="1"/>
-    <col min="10" max="11" width="11.7109375" customWidth="1"/>
-    <col min="12" max="12" width="42.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="8" width="23.7109375" customWidth="1"/>
+    <col min="9" max="10" width="21.7109375" customWidth="1"/>
+    <col min="11" max="12" width="11.7109375" customWidth="1"/>
+    <col min="13" max="13" width="112.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -646,164 +724,174 @@
         <v>11</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>61</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>62</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+        <v>61</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+        <v>62</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="L6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+        <v>61</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -813,17 +901,18 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="J7" s="1"/>
       <c r="K7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="L7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>62</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -831,23 +920,24 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="L8" t="s">
+        <v>61</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -857,49 +947,51 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="J9" s="1"/>
       <c r="K9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="L9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>62</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>61</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -909,49 +1001,51 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="J11" s="1"/>
       <c r="K11" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="L11" t="s">
+        <v>62</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="M11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>46</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="L12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+        <v>61</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -961,107 +1055,111 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="J13" s="1"/>
       <c r="K13" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="L13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+        <v>62</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>38</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="L14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>61</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="G15" s="1"/>
       <c r="H15" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="L15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+        <v>62</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>39</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="L16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+        <v>61</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1071,81 +1169,84 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="J17" s="1"/>
       <c r="K17" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="L17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+        <v>62</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="L18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+        <v>63</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="L19" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+        <v>61</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1155,17 +1256,18 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="J20" s="1"/>
       <c r="K20" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="L20" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
+        <v>62</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M20" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1176,46 +1278,48 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
-      <c r="K21" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L21" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="K21" s="1"/>
+      <c r="L21" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="L22" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
+        <v>61</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="M22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1225,107 +1329,111 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
-      <c r="J23" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="J23" s="1"/>
       <c r="K23" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="L23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+        <v>62</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L24" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
+        <v>61</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="G25" s="1"/>
       <c r="H25" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L25" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
+        <v>62</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="D26" s="1"/>
       <c r="E26" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="L26" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
+        <v>61</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M26" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1335,91 +1443,350 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="J27" s="1"/>
       <c r="K27" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L27" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
+        <v>62</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="D28" s="1"/>
       <c r="E28" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L28" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
+        <v>61</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-      <c r="G29" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="G29" s="1"/>
       <c r="H29" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L29" t="s">
-        <v>69</v>
+        <v>62</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="M30" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="M31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="M32" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="M33" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="M34" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="M35" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M36" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M37" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="M38" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="M39" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="63">
-    <mergeCell ref="A2:A29"/>
+  <mergeCells count="91">
+    <mergeCell ref="A2:A39"/>
     <mergeCell ref="B2:B29"/>
+    <mergeCell ref="B30:B39"/>
     <mergeCell ref="C2:C29"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="C30:C39"/>
+    <mergeCell ref="D2:D29"/>
+    <mergeCell ref="D30:D39"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="E6:E9"/>
@@ -1432,6 +1799,10 @@
     <mergeCell ref="E24:E25"/>
     <mergeCell ref="E26:E27"/>
     <mergeCell ref="E28:E29"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="E32:E35"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="E38:E39"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="F6:F9"/>
@@ -1444,21 +1815,37 @@
     <mergeCell ref="F24:F25"/>
     <mergeCell ref="F26:F27"/>
     <mergeCell ref="F28:F29"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="F32:F35"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="G4:G5"/>
     <mergeCell ref="G6:G9"/>
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G14:G15"/>
     <mergeCell ref="G16:G17"/>
     <mergeCell ref="G19:G21"/>
     <mergeCell ref="G22:G23"/>
+    <mergeCell ref="G24:G25"/>
     <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="G32:G35"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="H6:H9"/>
     <mergeCell ref="H10:H11"/>
     <mergeCell ref="H12:H13"/>
     <mergeCell ref="H16:H17"/>
     <mergeCell ref="H19:H21"/>
     <mergeCell ref="H22:H23"/>
     <mergeCell ref="H26:H27"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="H32:H35"/>
+    <mergeCell ref="H36:H37"/>
+    <mergeCell ref="H38:H39"/>
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="I8:I9"/>
     <mergeCell ref="I10:I11"/>
@@ -1467,7 +1854,23 @@
     <mergeCell ref="I19:I21"/>
     <mergeCell ref="I22:I23"/>
     <mergeCell ref="I26:I27"/>
-    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="I32:I35"/>
+    <mergeCell ref="I36:I37"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="J19:J21"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="J32:J35"/>
+    <mergeCell ref="J36:J37"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="K20:K21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
eliminate corrupted files from CMIP5-CORDEX
</commit_message>
<xml_diff>
--- a/catalog.xlsx
+++ b/catalog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="106">
   <si>
     <t>variable_id</t>
   </si>
@@ -118,6 +118,9 @@
     <t>CLMcom-Hereon</t>
   </si>
   <si>
+    <t>CNRM-MF</t>
+  </si>
+  <si>
     <t>HCLIMcom-SMHI</t>
   </si>
   <si>
@@ -184,6 +187,9 @@
     <t>ICON-CLM-202407-1-1</t>
   </si>
   <si>
+    <t>CNRM-ALADIN64E1</t>
+  </si>
+  <si>
     <t>REMO2020</t>
   </si>
   <si>
@@ -268,6 +274,9 @@
     <t>v20240920</t>
   </si>
   <si>
+    <t>v20250116</t>
+  </si>
+  <si>
     <t>v20241120</t>
   </si>
   <si>
@@ -286,6 +295,9 @@
     <t>['pr', 'tas', 'tasmax', 'tasmin']</t>
   </si>
   <si>
+    <t>['pr', 'psl', 'tasmax', 'tasmin']</t>
+  </si>
+  <si>
     <t>['pr', 'psl']</t>
   </si>
   <si>
@@ -299,6 +311,12 @@
   </si>
   <si>
     <t>['hurs', 'pr', 'prsn', 'ps', 'psl', 'tas', 'tasmax', 'tasmin', 'uas', 'vas']</t>
+  </si>
+  <si>
+    <t>['orog', 'areacella', 'rootd', 'sftlf']</t>
+  </si>
+  <si>
+    <t>['clt', 'evspsbl', 'hfls', 'hfss', 'hurs', 'od550aer', 'pr', 'psl', 'rlds', 'rlut', 'rsds', 'rsut', 'tas', 'tasmax', 'tasmin']</t>
   </si>
   <si>
     <t>['hurs', 'pr', 'prw', 'tas']</t>
@@ -671,7 +689,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -686,7 +704,7 @@
     <col min="7" max="8" width="23.7109375" customWidth="1"/>
     <col min="9" max="10" width="21.7109375" customWidth="1"/>
     <col min="11" max="12" width="11.7109375" customWidth="1"/>
-    <col min="13" max="13" width="112.7109375" customWidth="1"/>
+    <col min="13" max="13" width="128.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -747,28 +765,28 @@
         <v>20</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="M2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -780,22 +798,22 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="M3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -807,28 +825,28 @@
         <v>21</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M4" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -840,22 +858,22 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M5" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -867,28 +885,28 @@
         <v>22</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M6" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -903,13 +921,13 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M7" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -922,19 +940,19 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="M8" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -949,13 +967,13 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="M9" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -967,28 +985,28 @@
         <v>23</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="M10" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -1003,13 +1021,13 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M11" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -1021,28 +1039,28 @@
         <v>24</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M12" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -1057,13 +1075,13 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -1075,28 +1093,28 @@
         <v>25</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="M14" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -1108,22 +1126,22 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="M15" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -1135,28 +1153,28 @@
         <v>26</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M16" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -1171,13 +1189,13 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M17" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -1189,28 +1207,28 @@
         <v>27</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M18" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -1222,28 +1240,28 @@
         <v>28</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="M19" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -1258,13 +1276,13 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="M20" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -1280,10 +1298,10 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M21" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -1295,28 +1313,28 @@
         <v>29</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="M22" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -1331,13 +1349,13 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M23" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -1349,28 +1367,28 @@
         <v>30</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="M24" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -1382,22 +1400,22 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="M25" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -1409,28 +1427,28 @@
         <v>31</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="M26" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -1445,13 +1463,13 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="M27" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -1463,28 +1481,28 @@
         <v>32</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M28" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -1496,22 +1514,22 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M29" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -1529,28 +1547,28 @@
         <v>33</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M30" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -1565,13 +1583,13 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M31" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -1580,31 +1598,31 @@
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M32" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:13">
@@ -1619,13 +1637,13 @@
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M33" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:13">
@@ -1633,20 +1651,32 @@
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
+      <c r="E34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="K34" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M34" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:13">
@@ -1661,13 +1691,13 @@
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M35" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:13">
@@ -1675,32 +1705,20 @@
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
-      <c r="E36" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
       <c r="K36" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="M36" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:13">
@@ -1715,13 +1733,13 @@
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="M37" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:13">
@@ -1730,31 +1748,31 @@
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="M38" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:13">
@@ -1769,24 +1787,78 @@
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="M39" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J40" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="L39" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="M39" t="s">
-        <v>88</v>
+      <c r="K40" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M40" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M41" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="91">
-    <mergeCell ref="A2:A39"/>
+  <mergeCells count="97">
+    <mergeCell ref="A2:A41"/>
     <mergeCell ref="B2:B29"/>
-    <mergeCell ref="B30:B39"/>
+    <mergeCell ref="B30:B41"/>
     <mergeCell ref="C2:C29"/>
-    <mergeCell ref="C30:C39"/>
+    <mergeCell ref="C30:C41"/>
     <mergeCell ref="D2:D29"/>
-    <mergeCell ref="D30:D39"/>
+    <mergeCell ref="D30:D41"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="E6:E9"/>
@@ -1800,9 +1872,10 @@
     <mergeCell ref="E26:E27"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="E30:E31"/>
-    <mergeCell ref="E32:E35"/>
-    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="E34:E37"/>
     <mergeCell ref="E38:E39"/>
+    <mergeCell ref="E40:E41"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="F6:F9"/>
@@ -1816,9 +1889,10 @@
     <mergeCell ref="F26:F27"/>
     <mergeCell ref="F28:F29"/>
     <mergeCell ref="F30:F31"/>
-    <mergeCell ref="F32:F35"/>
-    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="F34:F37"/>
     <mergeCell ref="F38:F39"/>
+    <mergeCell ref="F40:F41"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="G6:G9"/>
@@ -1832,9 +1906,10 @@
     <mergeCell ref="G26:G27"/>
     <mergeCell ref="G28:G29"/>
     <mergeCell ref="G30:G31"/>
-    <mergeCell ref="G32:G35"/>
-    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="G34:G37"/>
     <mergeCell ref="G38:G39"/>
+    <mergeCell ref="G40:G41"/>
     <mergeCell ref="H6:H9"/>
     <mergeCell ref="H10:H11"/>
     <mergeCell ref="H12:H13"/>
@@ -1843,9 +1918,10 @@
     <mergeCell ref="H22:H23"/>
     <mergeCell ref="H26:H27"/>
     <mergeCell ref="H30:H31"/>
-    <mergeCell ref="H32:H35"/>
-    <mergeCell ref="H36:H37"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="H34:H37"/>
     <mergeCell ref="H38:H39"/>
+    <mergeCell ref="H40:H41"/>
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="I8:I9"/>
     <mergeCell ref="I10:I11"/>
@@ -1855,9 +1931,10 @@
     <mergeCell ref="I22:I23"/>
     <mergeCell ref="I26:I27"/>
     <mergeCell ref="I30:I31"/>
-    <mergeCell ref="I32:I35"/>
-    <mergeCell ref="I36:I37"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="I34:I37"/>
     <mergeCell ref="I38:I39"/>
+    <mergeCell ref="I40:I41"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="J8:J9"/>
     <mergeCell ref="J10:J11"/>
@@ -1867,9 +1944,10 @@
     <mergeCell ref="J22:J23"/>
     <mergeCell ref="J26:J27"/>
     <mergeCell ref="J30:J31"/>
-    <mergeCell ref="J32:J35"/>
-    <mergeCell ref="J36:J37"/>
+    <mergeCell ref="J32:J33"/>
+    <mergeCell ref="J34:J37"/>
     <mergeCell ref="J38:J39"/>
+    <mergeCell ref="J40:J41"/>
     <mergeCell ref="K20:K21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>